<commit_message>
add tab 39 report
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_39_rpt_PF_PortfolioForecastAll.xlsx
+++ b/backend/reports/xlsx/Tab_39_rpt_PF_PortfolioForecastAll.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleshapka/Development/github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FBE1294-CB86-C04C-8302-F561AC3CA0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB49EFE-314F-F748-B0CE-45F456EE3FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36920" yWindow="-21100" windowWidth="21600" windowHeight="37900" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="38020" yWindow="1900" windowWidth="34560" windowHeight="19700" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$G$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,16 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>{#date=d.date}</t>
   </si>
@@ -59,10 +50,106 @@
     <t>Project Name</t>
   </si>
   <si>
-    <t>{#fy=d.fiscal_year}</t>
-  </si>
-  <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+    <t>Project Recoveries Forecast by Area for as of {$date}</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name}</t>
+  </si>
+  <si>
+    <t>{$r1}</t>
+  </si>
+  <si>
+    <t>{#r=d.reportsByPortfolioWithTotals[i]}</t>
+  </si>
+  <si>
+    <t>{#r1=d.reportsByPortfolioWithTotals[i+1]}</t>
+  </si>
+  <si>
+    <t>Government Digital Experience (GDX Totals)</t>
+  </si>
+  <si>
+    <t>{$t.sum_of_q1_amount}</t>
+  </si>
+  <si>
+    <t>{$t.sum_of_q2_amount}</t>
+  </si>
+  <si>
+    <t>{$t.sum_of_q3_amount}</t>
+  </si>
+  <si>
+    <t>{$t.sum_of_q4_amount}</t>
+  </si>
+  <si>
+    <t>{$t.total}</t>
+  </si>
+  <si>
+    <t>{#t=d.grand_totals[0]}</t>
+  </si>
+  <si>
+    <t>{#p=d.reportsByPortfolioWithTotals[i].projects[i]}</t>
+  </si>
+  <si>
+    <t>{$p.project_number}</t>
+  </si>
+  <si>
+    <t>{#p1=d.reportsByPortfolioWithTotals[i].projects[i+1]}</t>
+  </si>
+  <si>
+    <t>{$p1}</t>
+  </si>
+  <si>
+    <t>{$p.project_name}</t>
+  </si>
+  <si>
+    <t>{$p.sum_of_q1_amount}</t>
+  </si>
+  <si>
+    <t>{$p.sum_of_q2_amount}</t>
+  </si>
+  <si>
+    <t>{$p.sum_of_q3_amount}</t>
+  </si>
+  <si>
+    <t>{$p.sum_of_q4_amount}</t>
+  </si>
+  <si>
+    <t>{$p.total}</t>
+  </si>
+  <si>
+    <t>{#s=d.reportsByPortfolioWithTotals[i].portfolio_totals}</t>
+  </si>
+  <si>
+    <t>{$s.sum_of_q1_amount}</t>
+  </si>
+  <si>
+    <t>{$s.sum_of_q2_amount}</t>
+  </si>
+  <si>
+    <t>{$s.sum_of_q3_amount}</t>
+  </si>
+  <si>
+    <t>{$s.sum_of_q4_amount}</t>
+  </si>
+  <si>
+    <t>{$s.total}</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name} Subtotals</t>
   </si>
 </sst>
 </file>
@@ -129,27 +216,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -192,60 +264,130 @@
       <right style="medium">
         <color rgb="FFBFBFBF"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
       <top style="medium">
         <color rgb="FFBFBFBF"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -626,10 +768,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -639,100 +781,184 @@
     <col min="3" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="19">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
+      <c r="G3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" thickBot="1">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="28">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="C2:I2" xr:uid="{0F20F7FF-D6FB-0145-BC76-92F810195548}"/>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>